<commit_message>
minor fixes and fullness factor
</commit_message>
<xml_diff>
--- a/code/output/data_pivot.xlsx
+++ b/code/output/data_pivot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>Rice (raw)</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>Energy</t>
+  </si>
+  <si>
+    <t>Fullness</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BJ33"/>
+  <dimension ref="A1:BJ34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6863,6 +6866,194 @@
         <v>1850</v>
       </c>
     </row>
+    <row r="34" spans="1:62">
+      <c r="A34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+      <c r="AM34">
+        <v>0</v>
+      </c>
+      <c r="AN34">
+        <v>0</v>
+      </c>
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>0</v>
+      </c>
+      <c r="AQ34">
+        <v>0</v>
+      </c>
+      <c r="AR34">
+        <v>0</v>
+      </c>
+      <c r="AS34">
+        <v>0</v>
+      </c>
+      <c r="AT34">
+        <v>0</v>
+      </c>
+      <c r="AU34">
+        <v>0</v>
+      </c>
+      <c r="AV34">
+        <v>0</v>
+      </c>
+      <c r="AW34">
+        <v>0</v>
+      </c>
+      <c r="AX34">
+        <v>0</v>
+      </c>
+      <c r="AY34">
+        <v>0</v>
+      </c>
+      <c r="AZ34">
+        <v>0</v>
+      </c>
+      <c r="BA34">
+        <v>0</v>
+      </c>
+      <c r="BB34">
+        <v>0</v>
+      </c>
+      <c r="BC34">
+        <v>0</v>
+      </c>
+      <c r="BD34">
+        <v>0</v>
+      </c>
+      <c r="BE34">
+        <v>0</v>
+      </c>
+      <c r="BF34">
+        <v>0</v>
+      </c>
+      <c r="BG34">
+        <v>0</v>
+      </c>
+      <c r="BH34">
+        <v>0</v>
+      </c>
+      <c r="BI34">
+        <v>0</v>
+      </c>
+      <c r="BJ34">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>